<commit_message>
modified:   calendar_events.xlsx 	modified:   punch_records.xlsx 	modified:   streamlit_app.py 	modified:   "\345\210\206\351\235\210\350\263\207\350\250\212.xlsx"
</commit_message>
<xml_diff>
--- a/calendar_events.xlsx
+++ b/calendar_events.xlsx
@@ -1,48 +1,62 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
-  <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="5">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
     <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
     <numFmt numFmtId="167" formatCode="YYYY-MM-DD"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -50,96 +64,18 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -218,6 +154,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -252,6 +189,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -286,20 +224,16 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -421,69 +355,71 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
+      <c r="A1" t="str">
+        <v>title</v>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>start</t>
-        </is>
+      <c r="B1" t="str">
+        <v>start</v>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>end</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>PA</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>45799</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>45799</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>GG</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="n">
-        <v>45799</v>
-      </c>
-      <c r="C3" s="3" t="n">
-        <v>45808</v>
+      <c r="C1" t="str">
+        <v>end</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:C1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>